<commit_message>
Implement document upload functionality
</commit_message>
<xml_diff>
--- a/data/building_code.xlsx
+++ b/data/building_code.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\dokuman_yonetim_sistemi\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB3D5785-39E5-4724-84D4-2013FAC13405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE108BF8-E7F6-426C-8705-466B85EBFD2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1042" yWindow="1042" windowWidth="18000" windowHeight="10433" xr2:uid="{5E7274F9-50BE-4897-B991-79E8EE958611}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{5E7274F9-50BE-4897-B991-79E8EE958611}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -165,10 +165,6 @@
     <t>EW10</t>
   </si>
   <si>
-    <t>EWB-10-Conditioning Building 
-(Small Scale Propellant Assembly)</t>
-  </si>
-  <si>
     <t>EW11</t>
   </si>
   <si>
@@ -196,9 +192,6 @@
     <t>GF02</t>
   </si>
   <si>
-    <t>GFB-02-Main Entrance Building (pedestrian)</t>
-  </si>
-  <si>
     <t>GF03</t>
   </si>
   <si>
@@ -208,9 +201,6 @@
     <t>GF04</t>
   </si>
   <si>
-    <t>GFB-04-Cafeteria (Dining Hall Building)</t>
-  </si>
-  <si>
     <t>GF05</t>
   </si>
   <si>
@@ -250,9 +240,6 @@
     <t>GF11</t>
   </si>
   <si>
-    <t>GFB-11-Security Tower (8 units)</t>
-  </si>
-  <si>
     <t>GF12</t>
   </si>
   <si>
@@ -316,9 +303,6 @@
     <t>GF14</t>
   </si>
   <si>
-    <t>GFB-14-Water Tank Building (Potable water)</t>
-  </si>
-  <si>
     <t>GF15</t>
   </si>
   <si>
@@ -358,10 +342,6 @@
     <t>IS02</t>
   </si>
   <si>
-    <t>ISB-02-Inert Material Storage Building
-(Incoming Inspection and Calibration)</t>
-  </si>
-  <si>
     <t>IS03</t>
   </si>
   <si>
@@ -420,6 +400,24 @@
   </si>
   <si>
     <t>description</t>
+  </si>
+  <si>
+    <t>GFB-02-Main Entrance Building &lt;pedestrian&gt;</t>
+  </si>
+  <si>
+    <t>GFB-04-Cafeteria &lt;Dining Hall Building&gt;</t>
+  </si>
+  <si>
+    <t>GFB-11-Security Tower &lt;8 units&gt;</t>
+  </si>
+  <si>
+    <t>GFB-14-Water Tank Building &lt;Potable water&gt;</t>
+  </si>
+  <si>
+    <t>EWB-10-Conditioning Building &lt;Small Scale Propellant Assembly&gt;</t>
+  </si>
+  <si>
+    <t>ISB-02-Inert Material Storage Building &lt;Incoming Inspection and Calibration&gt;</t>
   </si>
 </sst>
 </file>
@@ -455,8 +453,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F193D4-C93D-4637-BAC1-475720EA1592}">
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C64" sqref="C2:C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -783,516 +784,768 @@
     <col min="2" max="2" width="61.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C2" t="str">
+        <f>"INSERT INTO building_codes (code, description) VALUES ( '"&amp;A2&amp;"', '"&amp;B2&amp;"')"&amp;" ON CONFLICT(code) DO NOTHING;"</f>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GN00', 'General') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C64" si="0">"INSERT INTO building_codes (code, description) VALUES ( '"&amp;A3&amp;"', '"&amp;B3&amp;"')"&amp;" ON CONFLICT(code) DO NOTHING;"</f>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IN00', 'Infrastructure') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'MB00', 'Mobilisation') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES01', 'ESB-01-AP Storage Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES02', 'ESB-02-AP Storage Handling Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES03', 'ESB-03-Fuse Storage') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES04', 'ESB-04-Warhead Storage Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES05', 'ESB-05-Ammunition Storage Building-1') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES06', 'ESB-06-Ammunition Storage Building-2') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES07', 'ESB-07-Ammunition Storage Building-3') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES08', 'ESB-08-Ammunition Storage Building-4') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'ES09', 'ESB-09-Storage for Destruction') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW01', 'EWB-01-Hammer Mill Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW02', 'EWB-02-AP Storage and Conditioning Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW03', 'EWB-03-Mixer Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW04', 'EWB-04-Premix and Mixbowl Cleaning Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>32</v>
       </c>
       <c r="B18" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW05', 'EWB-05-Propellant Casting Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW06', 'EWB-06-Propellant Mandrel Disassembly Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>36</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW07', 'EWB-07-X-ray and Quality Control Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>38</v>
       </c>
       <c r="B21" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW08', 'EWB-08-Laboratory Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>40</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW09', 'EWB-09-Small Scale Propellant Assembly Firing Test') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>42</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW10', 'EWB-10-Conditioning Building &lt;Small Scale Propellant Assembly&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>44</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW11', 'EWB-11-Warhead Filling and Assembly Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW12', 'EWB-12-Warhead Press Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'EW13', 'EWB-13-Final Assembly Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF01', 'GFB-01-Main Entrance Check Point') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF02', 'GFB-02-Main Entrance Building &lt;pedestrian&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>52</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF03', 'GFB-03-Management_Administrative_R&amp;D Office ') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>54</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" t="s">
+        <v>123</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF04', 'GFB-04-Cafeteria &lt;Dining Hall Building&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+      <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF05', 'GFB-05-Health Center') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B32" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF06', 'GFB-06-Data Center') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+      <c r="B33" t="s">
         <v>60</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF07', 'GFB-07-Facility Maintanance Office and Workshop') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B34" t="s">
         <v>62</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF08', 'GFB-08-Fire Station') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B35" t="s">
         <v>64</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF09', 'GFB-09-Heating Plant') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+      <c r="B36" t="s">
         <v>66</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF10', 'GFB-10-Energetic Area Entrance Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF11', 'GFB-11-Security Tower &lt;8 units&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>68</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF12', 'GFB-12-Main Transformer Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>70</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B39" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13A', 'GFB-13A-Transformer Building-A') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>72</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B40" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13B', 'GFB-13B-Transformer Building-B') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>74</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13C', 'GFB-13C-Transformer Building-C') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>76</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B42" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13D', 'GFB-13D-Transformer Building-D') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>78</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13E', 'GFB-13E-Transformer Building-E') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>80</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B44" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13F', 'GFB-13F-Transformer Building-F') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>82</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B45" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13G', 'GFB-13G-Transformer Building-G') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>84</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B46" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13H', 'GFB-13H-Transformer Building-H') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
         <v>86</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B47" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'G13I', 'GFB-13I-Transformer Building-I') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
         <v>88</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF14', 'GFB-14-Water Tank Building &lt;Potable water&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
+      <c r="B49" t="s">
         <v>90</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF15', 'GFB-15-Fire Water Tank Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
+      <c r="B50" t="s">
         <v>92</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C50" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF16', 'GFB-16-Waste Water Purification Plant ') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="B51" t="s">
         <v>94</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C51" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF17', 'GFB-17-Industrial Waste Water Purification Plant ') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+      <c r="B52" t="s">
         <v>96</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C52" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF18', 'GFB-18-Temporary Waste Holding Area ') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C53" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'GF19', 'GFB-19-Main Entrance Logistics') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+      <c r="B54" t="s">
         <v>100</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C54" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IS01', 'ISB-01-Mixbowl_Mandrel and Tool Storage') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="B55" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IS02', 'ISB-02-Inert Material Storage Building &lt;Incoming Inspection and Calibration&gt;') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>102</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B56" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+      <c r="C56" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IS03', 'ISB-03-Chemical Material Storage Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>104</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B57" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="C57" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW01', 'IWB-01-Motor Case Production Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>106</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B58" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="C58" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW1A', 'IWB-01A-Motor Case Preform Production Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>108</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B59" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
+      <c r="C59" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW02', 'IWB-02-Motor Case Insulation and Composite') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>110</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B60" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
+      <c r="C60" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW03', 'IWB-03-Spray Application Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>112</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B61" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
+      <c r="C61" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW04', 'IWB-04-Control Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>114</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B62" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
+      <c r="C62" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW05', 'IWB-05-Small Scale Propellant Assembly Test Control') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>116</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B63" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
+      <c r="C63" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW06', 'IWB-06-Propellant Employee Office Building') ON CONFLICT(code) DO NOTHING;</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A64" t="s">
         <v>118</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B64" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>120</v>
-      </c>
-      <c r="B62" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>122</v>
-      </c>
-      <c r="B63" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>124</v>
-      </c>
-      <c r="B64" t="s">
-        <v>125</v>
+      <c r="C64" t="str">
+        <f t="shared" si="0"/>
+        <v>INSERT INTO building_codes (code, description) VALUES ( 'IW07', 'IWB-07-Warhead Employee Office Building') ON CONFLICT(code) DO NOTHING;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>